<commit_message>
add some config tables
</commit_message>
<xml_diff>
--- a/DataConfig/Entity.xlsx
+++ b/DataConfig/Entity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17745" windowHeight="7455"/>
+    <workbookView windowWidth="25230" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>场景配置表</t>
+    <t>Entity配置表</t>
   </si>
   <si>
     <t>Id</t>
@@ -34,7 +34,7 @@
     <t>string</t>
   </si>
   <si>
-    <t>场景编号</t>
+    <t>Entity编号</t>
   </si>
   <si>
     <t>策划备注</t>
@@ -53,6 +53,54 @@
   </si>
   <si>
     <t>Hero_XiaoBai</t>
+  </si>
+  <si>
+    <t>默认推进器</t>
+  </si>
+  <si>
+    <t>DefaultEngine</t>
+  </si>
+  <si>
+    <t>火箭推进器</t>
+  </si>
+  <si>
+    <t>RocketEngine</t>
+  </si>
+  <si>
+    <t>默认武器</t>
+  </si>
+  <si>
+    <t>DefaultWeapon</t>
+  </si>
+  <si>
+    <t>默认装甲</t>
+  </si>
+  <si>
+    <t>DefaultArmor</t>
+  </si>
+  <si>
+    <t>钢铁装甲</t>
+  </si>
+  <si>
+    <t>IronArmor</t>
+  </si>
+  <si>
+    <t>默认子弹</t>
+  </si>
+  <si>
+    <t>DefaultBolt</t>
+  </si>
+  <si>
+    <t>小明死亡特效</t>
+  </si>
+  <si>
+    <t>XiaoMingDeadEffect</t>
+  </si>
+  <si>
+    <t>小白死亡特效</t>
+  </si>
+  <si>
+    <t>XiaoBaiDeadEffect</t>
   </si>
 </sst>
 </file>
@@ -60,10 +108,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -74,7 +122,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -82,31 +129,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,21 +145,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,21 +153,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,9 +166,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,9 +213,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,15 +246,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,12 +275,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -245,37 +359,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,127 +449,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,20 +471,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -459,32 +496,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,6 +518,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -518,6 +546,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -526,10 +574,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -538,19 +586,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -559,112 +607,112 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,15 +1068,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1095,6 +1145,94 @@
       </c>
       <c r="D6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7">
+        <v>20000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8">
+        <v>20001</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9">
+        <v>30000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10">
+        <v>40000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11">
+        <v>40001</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12">
+        <v>50000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13">
+        <v>70000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14">
+        <v>70001</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>